<commit_message>
2.1.9: multiple bug fixes for Toronto
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -156,9 +156,6 @@
     <t>Palo Alto</t>
   </si>
   <si>
-    <t>Closed, Wheelchair Accessible, Women Only</t>
-  </si>
-  <si>
     <t>Noon</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>304 North 6th Street</t>
   </si>
   <si>
-    <t>Closed, Men Only</t>
-  </si>
-  <si>
     <t>Sunnyvale</t>
   </si>
   <si>
@@ -439,6 +433,12 @@
   </si>
   <si>
     <t>2700 Booksin Avenue</t>
+  </si>
+  <si>
+    <t>Closed, Men</t>
+  </si>
+  <si>
+    <t>Closed, Wheelchair Accessible, Women</t>
   </si>
 </sst>
 </file>
@@ -843,7 +843,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -906,16 +906,16 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
         <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>107</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -933,7 +933,7 @@
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>26</v>
@@ -947,10 +947,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
@@ -985,22 +985,22 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1012,7 +1012,7 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
         <v>26</v>
@@ -1026,16 +1026,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
@@ -1053,10 +1053,10 @@
         <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="Q5" s="2">
         <v>40465.831412037034</v>
@@ -1067,19 +1067,19 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
         <v>97</v>
       </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -1091,10 +1091,10 @@
         <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="Q6" s="2">
         <v>40830.646898148145</v>
@@ -1105,16 +1105,16 @@
         <v>0.4375</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -1132,7 +1132,7 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1184,16 +1184,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" t="s">
         <v>137</v>
-      </c>
-      <c r="D9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" t="s">
-        <v>139</v>
       </c>
       <c r="F9" t="s">
         <v>25</v>
@@ -1211,7 +1211,7 @@
         <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1228,16 +1228,16 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -1249,7 +1249,7 @@
         <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L10" t="s">
         <v>26</v>
@@ -1263,16 +1263,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1290,7 +1290,7 @@
         <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="Q11" s="2">
         <v>40328.022488425922</v>
@@ -1301,10 +1301,10 @@
         <v>0.75</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
@@ -1342,16 +1342,16 @@
         <v>0.8125</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -1380,16 +1380,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" t="s">
         <v>94</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>96</v>
       </c>
       <c r="F14" t="s">
         <v>25</v>
@@ -1407,10 +1407,10 @@
         <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="Q14" s="2">
         <v>40830.642939814818</v>
@@ -1421,10 +1421,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
@@ -1459,16 +1459,16 @@
         <v>0.78125</v>
       </c>
       <c r="B16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" t="s">
         <v>131</v>
       </c>
-      <c r="C16" t="s">
-        <v>133</v>
-      </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -1492,7 +1492,7 @@
         <v>26</v>
       </c>
       <c r="M16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q16" s="2">
         <v>40401.758726851855</v>
@@ -1503,16 +1503,16 @@
         <v>0.8125</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
         <v>44</v>
@@ -1530,7 +1530,7 @@
         <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q17" s="2">
         <v>40328.022523148145</v>
@@ -1541,7 +1541,7 @@
         <v>0.25</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
@@ -1576,19 +1576,19 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
         <v>127</v>
       </c>
-      <c r="C19" t="s">
-        <v>129</v>
-      </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
@@ -1609,7 +1609,7 @@
         <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="2">
         <v>40328.022499999999</v>
@@ -1620,16 +1620,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
         <v>113</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>115</v>
       </c>
       <c r="F20" t="s">
         <v>25</v>
@@ -1647,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="K20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L20" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="Q20" s="2">
         <v>40830.650578703702</v>
@@ -1661,10 +1661,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1702,13 +1702,13 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -1746,10 +1746,10 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
@@ -1784,16 +1784,16 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3">
         <v>0.4236111111111111</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
         <v>44</v>
@@ -1814,7 +1814,7 @@
         <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q24" s="2">
         <v>40822.963599537034</v>
@@ -1825,16 +1825,16 @@
         <v>0.75</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F25" t="s">
         <v>25</v>
@@ -1852,7 +1852,7 @@
         <v>25</v>
       </c>
       <c r="K25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L25" t="s">
         <v>26</v>
@@ -1863,19 +1863,19 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" t="s">
-        <v>128</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>47</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -1893,7 +1893,7 @@
         <v>25</v>
       </c>
       <c r="K26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
@@ -1907,16 +1907,16 @@
         <v>0.84375</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" t="s">
         <v>116</v>
-      </c>
-      <c r="D27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
@@ -1937,7 +1937,7 @@
         <v>36</v>
       </c>
       <c r="L27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q27" s="2">
         <v>40830.644212962965</v>
@@ -1945,19 +1945,19 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -1986,16 +1986,16 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
         <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -2013,7 +2013,7 @@
         <v>33</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q29" s="2">
         <v>40914.89943287037</v>
@@ -2024,16 +2024,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
         <v>32</v>
@@ -2051,7 +2051,7 @@
         <v>32</v>
       </c>
       <c r="L30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q30" s="2">
         <v>40328.022523148145</v>
@@ -2059,19 +2059,19 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
         <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>51</v>
       </c>
       <c r="F31" t="s">
         <v>25</v>
@@ -2089,7 +2089,7 @@
         <v>25</v>
       </c>
       <c r="K31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L31" t="s">
         <v>23</v>
@@ -2103,16 +2103,16 @@
         <v>0.75</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F32" t="s">
         <v>44</v>
@@ -2138,19 +2138,19 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
         <v>119</v>
       </c>
-      <c r="C33" t="s">
-        <v>121</v>
-      </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F33" t="s">
         <v>32</v>
@@ -2168,7 +2168,7 @@
         <v>32</v>
       </c>
       <c r="L33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q33" s="2">
         <v>40725.859525462962</v>
@@ -2179,16 +2179,16 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s">
         <v>25</v>
@@ -2220,10 +2220,10 @@
         <v>0.8125</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>

</xml_diff>